<commit_message>
last version where all modules work
</commit_message>
<xml_diff>
--- a/contragent.xlsx
+++ b/contragent.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mark\Desktop\excel_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\malts_000\Desktop\excel_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="75">
   <si>
     <t>Код</t>
   </si>
@@ -202,6 +202,48 @@
   </si>
   <si>
     <t>Индивидуальный предприниматель Рудакова Елена Вениаминовна</t>
+  </si>
+  <si>
+    <t>киселева</t>
+  </si>
+  <si>
+    <t>ИП Киселева Г.В.</t>
+  </si>
+  <si>
+    <t>sample_contract_code</t>
+  </si>
+  <si>
+    <t>b00010213</t>
+  </si>
+  <si>
+    <t>Индивидуальный предприниматель Магкаева Алина Ацамазовна</t>
+  </si>
+  <si>
+    <t>модуль</t>
+  </si>
+  <si>
+    <t>agold</t>
+  </si>
+  <si>
+    <t>estet</t>
+  </si>
+  <si>
+    <t>klyuvenkov</t>
+  </si>
+  <si>
+    <t>magia</t>
+  </si>
+  <si>
+    <t>neolog</t>
+  </si>
+  <si>
+    <t>ferrum</t>
+  </si>
+  <si>
+    <t>Индивидуальный предприниматель Магкаева Алина Ацамазовна</t>
+  </si>
+  <si>
+    <t>киселёва</t>
   </si>
 </sst>
 </file>
@@ -226,7 +268,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -249,13 +291,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -594,300 +648,405 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14:F14"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="30.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="99.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="99.5703125" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+    <col min="7" max="7" width="40.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>58</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="1">
+      <c r="F2" s="1">
         <v>9866</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="G2" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>11</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1"/>
+      <c r="C4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <v>10081</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="G4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1">
         <v>10158</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>59</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="1">
         <v>10074</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>49</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="E7" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="1">
+      <c r="F7" s="1">
         <v>10162</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="1">
+      <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="1">
+      <c r="F9" s="1">
         <v>9795</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>57</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="1">
         <v>10174</v>
       </c>
-      <c r="F10" s="1" t="s">
+      <c r="G10" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="E11" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="1">
+      <c r="F11" s="1">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>50</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="E12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E12" s="1">
+      <c r="F12" s="1">
         <v>10080</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="E13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="E13" s="1">
+      <c r="F13" s="1">
         <v>14</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="G13" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>60</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E14" s="1">
+      <c r="E14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="1">
         <v>10174</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
         <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>61</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="2">
+        <v>10519</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F16" s="1">
+        <v>10074</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>74</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F17" s="2">
+        <v>10519</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>